<commit_message>
Obróbka danych : ))
</commit_message>
<xml_diff>
--- a/Direct-taxes.xlsx
+++ b/Direct-taxes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Web Deposit\unitD4\TAXATION TRENDS DATA 2025\Indicators\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RPiSm\Programowanie w R\Analiza-symulacyjna\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB4C6FF-3FBF-4539-A5A3-856664C32BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7255E55A-22A1-4815-9237-EAB1898DAE12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C640BE43-3FC8-4301-B911-D7B3FF125D99}"/>
+    <workbookView xWindow="5410" yWindow="2580" windowWidth="19200" windowHeight="9970" xr2:uid="{C640BE43-3FC8-4301-B911-D7B3FF125D99}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 13" sheetId="1" r:id="rId1"/>
@@ -40919,7 +40919,7 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -40935,9 +40935,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Pakiet Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -40975,7 +40975,7 @@
         <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Pakiet Office">
       <a:majorFont>
         <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
@@ -41081,7 +41081,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Pakiet Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -41253,8 +41253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88FBD315-2D63-457B-A763-48825C542045}">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -43151,7 +43151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAB2273-4C46-46D7-94D7-ECE92787F695}">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView zoomScale="73" workbookViewId="0">
       <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
@@ -45049,7 +45049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD6B51A8-3E00-4CDD-9888-A9E6BEA1F8D7}">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
@@ -46947,7 +46947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A11A4450-B38C-4058-9D74-6A7275A53FBC}">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="95" workbookViewId="0">
       <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
@@ -48845,7 +48845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC6FBAA-41BA-44DA-889F-1C8217E71CEA}">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>

</xml_diff>